<commit_message>
Started work on visual prototype
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45e720c463866f42/School/4th Year/IndProject/Shaders-For-Scientific-Visualisation-Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF320710-BC06-4E51-90A0-DED563C9ED82}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A916B4-D775-4739-A68A-3DE6F5679A75}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="375" yWindow="345" windowWidth="28770" windowHeight="15480" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Individual Project Time Log</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>Reorganised project, started working on visual prototype</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -248,7 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,6 +267,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -566,7 +573,7 @@
   <dimension ref="B2:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +582,7 @@
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="51.5703125" customWidth="1"/>
+    <col min="6" max="6" width="59.140625" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,15 +618,19 @@
       <c r="C4" s="3">
         <v>2.5694444444444447E-2</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>0.26527777777777778</v>
+      </c>
       <c r="E4" s="11">
         <f>D4-C4</f>
-        <v>-2.5694444444444447E-2</v>
-      </c>
-      <c r="F4" s="11"/>
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="H4" s="12">
         <f>SUM(E4:E100)</f>
-        <v>-2.5694444444444447E-2</v>
+        <v>0.23958333333333334</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implemented remote rendering tests:  - Added package-lock to gitignore  - Refactored ExampleWidget into SSVRenderWidget  - Implemented basic SSVCanvas class for managing the renderer and widget  - Implemented skeleton jupyter widget (model, view, etc...)  - Implemented logging wrapper  - Implemented example moderngl renderer  - Added example code to the introduction.ipynb notebook  - Added meeting minutes from 2023-10-03  - Added testing code for moderngl threading  - Other small changes + refactoring
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45e720c463866f42/School/4th Year/IndProject/Shaders-For-Scientific-Visualisation-Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29A916B4-D775-4739-A68A-3DE6F5679A75}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EF9741C-8002-46FC-B490-44009F569ADA}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="375" yWindow="345" windowWidth="28770" windowHeight="15480" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Individual Project Time Log</t>
   </si>
@@ -60,6 +60,30 @@
   </si>
   <si>
     <t>Reorganised project, started working on visual prototype</t>
+  </si>
+  <si>
+    <t>Weekly meeting</t>
+  </si>
+  <si>
+    <t>Updated meeting minutes, did some more research</t>
+  </si>
+  <si>
+    <t>Researched different graphics and plotting libraries, and example use cases</t>
+  </si>
+  <si>
+    <t>Experimented with headless OpenGL, researched libraries, prepared more test data</t>
+  </si>
+  <si>
+    <t>Prepared slides, continued research into Widgets and H264 streaming</t>
+  </si>
+  <si>
+    <t>Meeting minutes</t>
+  </si>
+  <si>
+    <t>Integrated Jupyter widget template</t>
+  </si>
+  <si>
+    <t>Implemented prototype of the Jupyter widget which integrates an OpenGL renderer</t>
   </si>
 </sst>
 </file>
@@ -237,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -252,6 +276,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AAD46A-3194-4130-A472-583034294978}">
   <dimension ref="B2:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,106 +647,178 @@
         <v>0.26527777777777778</v>
       </c>
       <c r="E4" s="11">
-        <f>D4-C4</f>
+        <f>IF(D4-C4&lt;0, D4-C4+1, D4-C4)</f>
         <v>0.23958333333333334</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="14">
         <f>SUM(E4:E100)</f>
-        <v>0.23958333333333334</v>
+        <v>1.2965277777777779</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="2">
+        <v>45195</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.625</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.65763888888888888</v>
+      </c>
       <c r="E5" s="11">
-        <f t="shared" ref="E5:E68" si="0">D5-C5</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="11"/>
+        <f t="shared" ref="E5:E68" si="0">IF(D5-C5&lt;0, D5-C5+1, D5-C5)</f>
+        <v>3.2638888888888884E-2</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="2">
+        <v>45196</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.21041666666666667</v>
+      </c>
       <c r="E6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="11"/>
+        <v>4.3750000000000011E-2</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
+      <c r="B7" s="2">
+        <v>45196</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.12986111111111112</v>
+      </c>
       <c r="E7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>0.20208333333333339</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="2">
+        <v>45200</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.25625000000000003</v>
+      </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="11"/>
+        <v>0.21458333333333338</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="2">
+        <v>45202</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.17013888888888887</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.28125</v>
+      </c>
       <c r="E9" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="11"/>
+        <v>0.11111111111111113</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
+      <c r="B10" s="2">
+        <v>45202</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.5625</v>
+      </c>
       <c r="E10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="11"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
+      <c r="B11" s="2">
+        <v>45204</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.1125</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.1875</v>
+      </c>
       <c r="E11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="11"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="2">
+        <v>45206</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.33402777777777781</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.4548611111111111</v>
+      </c>
       <c r="E12" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="11"/>
+        <v>0.12083333333333329</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="2">
+        <v>45209</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.24930555555555556</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.48541666666666666</v>
+      </c>
       <c r="E13" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="11"/>
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -1278,7 +1375,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="4"/>
       <c r="E69" s="11">
-        <f t="shared" ref="E69:E100" si="1">D69-C69</f>
+        <f t="shared" ref="E69:E100" si="1">IF(D69-C69&lt;0, D69-C69+1, D69-C69)</f>
         <v>0</v>
       </c>
       <c r="F69" s="11"/>
@@ -1587,7 +1684,7 @@
       <c r="B100" s="5"/>
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
-      <c r="E100" s="12">
+      <c r="E100" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Updated notes:  - Added meeting minutes from previous meetings  - Added notes on various experiments and ideas  - Updated timelog
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45e720c463866f42/School/4th Year/IndProject/Shaders-For-Scientific-Visualisation-Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EF9741C-8002-46FC-B490-44009F569ADA}"/>
+  <xr:revisionPtr revIDLastSave="137" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75435B9F-5B2F-456B-865B-508DCB41CE70}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Individual Project Time Log</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>Implemented prototype of the Jupyter widget which integrates an OpenGL renderer</t>
+  </si>
+  <si>
+    <t>Worked towards multiprocess implementation, researched preprocessing</t>
+  </si>
+  <si>
+    <t>Implemented render process</t>
+  </si>
+  <si>
+    <t>Fixed build system, implemented watchdog, released build to PyPi</t>
+  </si>
+  <si>
+    <t>Meeting minutes &amp; Shader preprocessing work</t>
   </si>
 </sst>
 </file>
@@ -597,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AAD46A-3194-4130-A472-583034294978}">
   <dimension ref="B2:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +667,7 @@
       </c>
       <c r="H4" s="14">
         <f>SUM(E4:E100)</f>
-        <v>1.2965277777777779</v>
+        <v>2.5506944444444444</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -821,74 +833,130 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="2">
+        <v>45213</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.79236111111111107</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0.84166666666666667</v>
+      </c>
       <c r="E14" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="11"/>
+        <v>4.9305555555555602E-2</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="2">
+        <v>45216</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0.57638888888888895</v>
+      </c>
       <c r="E15" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="11"/>
+        <v>0.19583333333333341</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="2">
+        <v>45216</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.22222222222222221</v>
+      </c>
       <c r="E16" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="11"/>
+        <v>0.26388888888888884</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="2">
+        <v>45223</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E17" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="11"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="E18" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="11"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="2">
+        <v>45234</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.6118055555555556</v>
+      </c>
       <c r="E19" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="11"/>
+        <v>0.44513888888888897</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="2">
+        <v>45237</v>
+      </c>
+      <c r="C20" s="3">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.34166666666666662</v>
+      </c>
       <c r="E20" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="11"/>
+        <v>0.2583333333333333</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>

</xml_diff>

<commit_message>
Progress on the implementation chapter of the dissertation:  - First draft of most of the sections I wanted to discuss in the implementation of the dissertation  - Added a few diagrams  - Fixed some formatting issues with Latex & added JS/GLSL support to the syntax highlighter
</commit_message>
<xml_diff>
--- a/Timelog.xlsx
+++ b/Timelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45e720c463866f42/School/4th Year/IndProject/Shaders-For-Scientific-Visualisation-Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75435B9F-5B2F-456B-865B-508DCB41CE70}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="8_{2FBEDC51-3AE3-4D31-84D2-A590B54BB3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E5BD5E0-FB20-4BBA-B0D8-EC10391A274B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
+    <workbookView minimized="1" xWindow="2250" yWindow="1140" windowWidth="22830" windowHeight="12900" xr2:uid="{10544DDD-4804-44DF-9FAF-37CA0C5D2071}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Individual Project Time Log</t>
   </si>
@@ -96,6 +96,51 @@
   </si>
   <si>
     <t>Meeting minutes &amp; Shader preprocessing work</t>
+  </si>
+  <si>
+    <t>Work on shader preprocessing</t>
+  </si>
+  <si>
+    <t>Completed shader preprocessing</t>
+  </si>
+  <si>
+    <t>Multi-pass/multi-buffer api design &amp; research</t>
+  </si>
+  <si>
+    <t>Multi-pass/multi-buffer api implementation</t>
+  </si>
+  <si>
+    <t>Multi-pass/multi-buffer api implementation &amp; widget improvements</t>
+  </si>
+  <si>
+    <t>Multi-pass rendering</t>
+  </si>
+  <si>
+    <t>Renderdoc integration &amp; geometry shaders</t>
+  </si>
+  <si>
+    <t>Finished implementing textures &amp; updated documentation</t>
+  </si>
+  <si>
+    <t>Fixed geometry shaders and various other bugs. Prepared a new release</t>
+  </si>
+  <si>
+    <t>Camera bugfixes &amp; UI library implementation</t>
+  </si>
+  <si>
+    <t>Performance enhancements &amp; Video streaming</t>
+  </si>
+  <si>
+    <t>Linux bugfixes</t>
+  </si>
+  <si>
+    <t>DEM Terrain demo</t>
+  </si>
+  <si>
+    <t>Documentation improvements &amp; preparation for user testing</t>
+  </si>
+  <si>
+    <t>Implemented image saving</t>
   </si>
 </sst>
 </file>
@@ -311,9 +356,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -351,7 +396,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -457,7 +502,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +644,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -609,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AAD46A-3194-4130-A472-583034294978}">
   <dimension ref="B2:H100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +712,7 @@
       </c>
       <c r="H4" s="14">
         <f>SUM(E4:E100)</f>
-        <v>2.5506944444444444</v>
+        <v>6.7069444444444457</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -959,164 +1004,292 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="2">
+        <v>45239</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.7284722222222223</v>
+      </c>
       <c r="E21" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="11"/>
+        <v>0.17291666666666672</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="2">
+        <v>45241</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.74097222222222225</v>
+      </c>
       <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="11"/>
+        <v>0.43541666666666673</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
+      <c r="B23" s="2">
+        <v>45250</v>
+      </c>
+      <c r="C23" s="3">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D23" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="11"/>
+        <v>0.125</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
+      <c r="B24" s="2">
+        <v>45257</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="E24" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="11"/>
+        <f>IF(D24-C24&lt;0, D24-C24+1, D24-C24)</f>
+        <v>0.1875</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="2">
+        <v>45261</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.57222222222222219</v>
+      </c>
       <c r="E25" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="11"/>
+        <f>IF(D25-C25&lt;0, D25-C25+1, D25-C25)</f>
+        <v>0.19722222222222219</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
+      <c r="B26" s="2">
+        <v>45262</v>
+      </c>
+      <c r="C26" s="3">
+        <v>0.32708333333333334</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0.5180555555555556</v>
+      </c>
       <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="11"/>
+        <v>0.19097222222222227</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
+      <c r="B27" s="2">
+        <v>45265</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="11"/>
+        <v>0.25</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
+      <c r="B28" s="2">
+        <v>45266</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0.53472222222222221</v>
+      </c>
       <c r="E28" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="11"/>
+        <v>0.14930555555555552</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
+      <c r="B29" s="2">
+        <v>45267</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="E29" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="11"/>
+        <v>0.22916666666666663</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
+      <c r="B30" s="2">
+        <v>45302</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="E30" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="11"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="B31" s="2">
+        <v>45303</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="E31" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="11"/>
+        <v>0.5625</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
+      <c r="B32" s="2">
+        <v>45312</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E32" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="11"/>
+        <v>0.43749999999999994</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
+      <c r="B33" s="2">
+        <v>45317</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0.14583333333333334</v>
+      </c>
       <c r="E33" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F33" s="11"/>
+        <v>0.125</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
+      <c r="B34" s="2">
+        <v>45321</v>
+      </c>
+      <c r="C34" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="E34" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F34" s="11"/>
+        <v>0.22916666666666674</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
+      <c r="B35" s="2">
+        <v>45328</v>
+      </c>
+      <c r="C35" s="3">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0.5625</v>
+      </c>
       <c r="E35" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F35" s="11"/>
+        <v>0.35416666666666663</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
+      <c r="B36" s="2">
+        <v>45332</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D36" s="4">
+        <v>5.2083333333333336E-2</v>
+      </c>
       <c r="E36" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F36" s="11"/>
+        <v>0.21875</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>

</xml_diff>